<commit_message>
cambios en crono antiguo
</commit_message>
<xml_diff>
--- a/PREGAME/1. ELICITACIÓN/1.2 Cronograma/Cronograma_A&D_G1_V02.xlsx
+++ b/PREGAME/1. ELICITACIÓN/1.2 Cronograma/Cronograma_A&D_G1_V02.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\David\Universidad\Universidad\5 Semestre\Análisis y diseño\15035_G1_ADSW\PREGAME\1. ELICITACIÓN\1.2 Cronograma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Documentos\Cuarto Semestre\Analisis\15035_G1_ADSW\PREGAME\1. ELICITACIÓN\1.2 Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C489682-74B5-4D86-B427-A4253583B62E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104A3B8E-273B-49EB-B977-7DD21FBB0D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GR03-Gantt_proyecto-V001-30-06-" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="123">
   <si>
     <t>Cronograma Proyecto InClass</t>
   </si>
@@ -399,10 +399,16 @@
     <t>Desarrollo de Modulo de Tutorias (IC006, IC009</t>
   </si>
   <si>
-    <t>Desarrollo de Modulo de Usuarios y Cursos (IC001, IC002, IC003, IC004, IC007, IC013)</t>
-  </si>
-  <si>
     <t>Desarrollo de Modulo de Calificaciones (IC008, IC0011)</t>
+  </si>
+  <si>
+    <t>Desarrollo de Modulo de Usuarios y Cursos (IC001)</t>
+  </si>
+  <si>
+    <t>Correccion de errores</t>
+  </si>
+  <si>
+    <t>2 días</t>
   </si>
 </sst>
 </file>
@@ -919,10 +925,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:Y94"/>
+  <dimension ref="A1:Y95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="G73" sqref="G73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" outlineLevelRow="3"/>
@@ -2129,10 +2135,10 @@
         <v>45267</v>
       </c>
       <c r="F59" s="33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G59" s="30" t="s">
-        <v>85</v>
+        <v>13</v>
       </c>
       <c r="H59" s="40"/>
       <c r="I59" s="6"/>
@@ -2266,11 +2272,11 @@
       <c r="E63" s="44">
         <v>45270</v>
       </c>
-      <c r="F63" s="45">
-        <v>0</v>
+      <c r="F63" s="33">
+        <v>1</v>
       </c>
       <c r="G63" s="30" t="s">
-        <v>85</v>
+        <v>13</v>
       </c>
       <c r="H63" s="31"/>
       <c r="I63" s="1"/>
@@ -2291,11 +2297,11 @@
       <c r="E64" s="44">
         <v>45271</v>
       </c>
-      <c r="F64" s="45">
-        <v>0</v>
+      <c r="F64" s="33">
+        <v>1</v>
       </c>
       <c r="G64" s="30" t="s">
-        <v>85</v>
+        <v>13</v>
       </c>
       <c r="H64" s="31"/>
       <c r="I64" s="1"/>
@@ -2316,11 +2322,11 @@
       <c r="E65" s="44">
         <v>45303</v>
       </c>
-      <c r="F65" s="45">
-        <v>0</v>
+      <c r="F65" s="33">
+        <v>1</v>
       </c>
       <c r="G65" s="30" t="s">
-        <v>85</v>
+        <v>13</v>
       </c>
       <c r="H65" s="31"/>
       <c r="I65" s="1"/>
@@ -2381,11 +2387,11 @@
       <c r="E68" s="44">
         <v>45304</v>
       </c>
-      <c r="F68" s="45">
-        <v>0</v>
+      <c r="F68" s="33">
+        <v>1</v>
       </c>
       <c r="G68" s="30" t="s">
-        <v>85</v>
+        <v>13</v>
       </c>
       <c r="H68" s="31"/>
       <c r="I68" s="1"/>
@@ -2406,11 +2412,11 @@
       <c r="E69" s="44">
         <v>45305</v>
       </c>
-      <c r="F69" s="45">
-        <v>0</v>
+      <c r="F69" s="33">
+        <v>1</v>
       </c>
       <c r="G69" s="30" t="s">
-        <v>85</v>
+        <v>13</v>
       </c>
       <c r="H69" s="31"/>
       <c r="I69" s="1"/>
@@ -2444,9 +2450,9 @@
       <c r="X70" s="1"/>
       <c r="Y70" s="1"/>
     </row>
-    <row r="71" spans="1:25" ht="31.5" customHeight="1">
+    <row r="71" spans="1:25" ht="20.25" customHeight="1">
       <c r="A71" s="66" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B71" s="31" t="s">
         <v>97</v>
@@ -2460,120 +2466,120 @@
       <c r="E71" s="44">
         <v>45299</v>
       </c>
-      <c r="F71" s="45">
-        <v>0</v>
+      <c r="F71" s="33">
+        <v>1</v>
       </c>
       <c r="G71" s="30" t="s">
-        <v>85</v>
+        <v>13</v>
       </c>
       <c r="H71" s="31"/>
       <c r="I71" s="1"/>
     </row>
-    <row r="72" spans="1:25" ht="15" customHeight="1">
-      <c r="A72" s="52" t="s">
-        <v>99</v>
+    <row r="72" spans="1:25" ht="21.75" customHeight="1">
+      <c r="A72" s="66" t="s">
+        <v>121</v>
       </c>
       <c r="B72" s="31" t="s">
         <v>100</v>
       </c>
       <c r="C72" s="31" t="s">
-        <v>68</v>
+        <v>122</v>
       </c>
       <c r="D72" s="44">
-        <v>45300</v>
+        <v>45301</v>
       </c>
       <c r="E72" s="44">
-        <v>45300</v>
-      </c>
-      <c r="F72" s="45">
-        <v>0</v>
+        <v>45302</v>
+      </c>
+      <c r="F72" s="33">
+        <v>1</v>
       </c>
       <c r="G72" s="30" t="s">
-        <v>85</v>
+        <v>13</v>
       </c>
       <c r="H72" s="31"/>
       <c r="I72" s="1"/>
     </row>
     <row r="73" spans="1:25" ht="15" customHeight="1">
-      <c r="A73" s="31"/>
-      <c r="B73" s="31"/>
-      <c r="C73" s="31"/>
-      <c r="D73" s="44"/>
-      <c r="E73" s="44"/>
-      <c r="F73" s="45"/>
-      <c r="G73" s="30"/>
+      <c r="A73" s="52" t="s">
+        <v>99</v>
+      </c>
+      <c r="B73" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="C73" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="D73" s="44">
+        <v>45300</v>
+      </c>
+      <c r="E73" s="44">
+        <v>45300</v>
+      </c>
+      <c r="F73" s="33">
+        <v>1</v>
+      </c>
+      <c r="G73" s="30" t="s">
+        <v>13</v>
+      </c>
       <c r="H73" s="31"/>
       <c r="I73" s="1"/>
     </row>
     <row r="74" spans="1:25" ht="15" customHeight="1">
-      <c r="A74" s="48" t="s">
+      <c r="A74" s="31"/>
+      <c r="B74" s="31"/>
+      <c r="C74" s="31"/>
+      <c r="D74" s="44"/>
+      <c r="E74" s="44"/>
+      <c r="F74" s="45"/>
+      <c r="G74" s="30"/>
+      <c r="H74" s="31"/>
+      <c r="I74" s="1"/>
+    </row>
+    <row r="75" spans="1:25" ht="15" customHeight="1">
+      <c r="A75" s="48" t="s">
         <v>101</v>
       </c>
-      <c r="B74" s="49"/>
-      <c r="C74" s="49"/>
-      <c r="D74" s="49"/>
-      <c r="E74" s="49"/>
-      <c r="F74" s="49"/>
-      <c r="G74" s="50"/>
-      <c r="H74" s="49"/>
-      <c r="I74" s="1"/>
-      <c r="J74" s="1"/>
-      <c r="K74" s="1"/>
-      <c r="L74" s="1"/>
-      <c r="M74" s="1"/>
-      <c r="N74" s="1"/>
-      <c r="O74" s="1"/>
-      <c r="P74" s="1"/>
-      <c r="Q74" s="1"/>
-      <c r="R74" s="1"/>
-      <c r="S74" s="1"/>
-      <c r="T74" s="1"/>
-      <c r="U74" s="1"/>
-      <c r="V74" s="1"/>
-      <c r="W74" s="1"/>
-      <c r="X74" s="1"/>
-      <c r="Y74" s="1"/>
-    </row>
-    <row r="75" spans="1:25" ht="15" customHeight="1">
-      <c r="A75" s="31" t="s">
+      <c r="B75" s="49"/>
+      <c r="C75" s="49"/>
+      <c r="D75" s="49"/>
+      <c r="E75" s="49"/>
+      <c r="F75" s="49"/>
+      <c r="G75" s="50"/>
+      <c r="H75" s="49"/>
+      <c r="I75" s="1"/>
+      <c r="J75" s="1"/>
+      <c r="K75" s="1"/>
+      <c r="L75" s="1"/>
+      <c r="M75" s="1"/>
+      <c r="N75" s="1"/>
+      <c r="O75" s="1"/>
+      <c r="P75" s="1"/>
+      <c r="Q75" s="1"/>
+      <c r="R75" s="1"/>
+      <c r="S75" s="1"/>
+      <c r="T75" s="1"/>
+      <c r="U75" s="1"/>
+      <c r="V75" s="1"/>
+      <c r="W75" s="1"/>
+      <c r="X75" s="1"/>
+      <c r="Y75" s="1"/>
+    </row>
+    <row r="76" spans="1:25" ht="15" customHeight="1">
+      <c r="A76" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="B75" s="53" t="s">
+      <c r="B76" s="53" t="s">
         <v>97</v>
       </c>
-      <c r="C75" s="31" t="s">
+      <c r="C76" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="D75" s="44">
+      <c r="D76" s="44">
         <v>45308</v>
       </c>
-      <c r="E75" s="44">
+      <c r="E76" s="44">
         <v>45313</v>
-      </c>
-      <c r="F75" s="45">
-        <v>0</v>
-      </c>
-      <c r="G75" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="H75" s="31"/>
-      <c r="I75" s="1"/>
-    </row>
-    <row r="76" spans="1:25" ht="15" customHeight="1">
-      <c r="A76" s="52" t="s">
-        <v>102</v>
-      </c>
-      <c r="B76" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="C76" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="D76" s="44">
-        <v>45314</v>
-      </c>
-      <c r="E76" s="44">
-        <v>45314</v>
       </c>
       <c r="F76" s="45">
         <v>0</v>
@@ -2585,101 +2591,85 @@
       <c r="I76" s="1"/>
     </row>
     <row r="77" spans="1:25" ht="15" customHeight="1">
-      <c r="A77" s="52"/>
-      <c r="B77" s="31"/>
-      <c r="C77" s="31"/>
-      <c r="D77" s="44"/>
-      <c r="E77" s="44"/>
-      <c r="F77" s="45"/>
-      <c r="G77" s="30"/>
+      <c r="A77" s="52" t="s">
+        <v>102</v>
+      </c>
+      <c r="B77" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="C77" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="D77" s="44">
+        <v>45314</v>
+      </c>
+      <c r="E77" s="44">
+        <v>45314</v>
+      </c>
+      <c r="F77" s="45">
+        <v>0</v>
+      </c>
+      <c r="G77" s="30" t="s">
+        <v>85</v>
+      </c>
       <c r="H77" s="31"/>
       <c r="I77" s="1"/>
     </row>
     <row r="78" spans="1:25" ht="15" customHeight="1">
-      <c r="A78" s="54" t="s">
+      <c r="A78" s="52"/>
+      <c r="B78" s="31"/>
+      <c r="C78" s="31"/>
+      <c r="D78" s="44"/>
+      <c r="E78" s="44"/>
+      <c r="F78" s="45"/>
+      <c r="G78" s="30"/>
+      <c r="H78" s="31"/>
+      <c r="I78" s="1"/>
+    </row>
+    <row r="79" spans="1:25" ht="15" customHeight="1">
+      <c r="A79" s="54" t="s">
         <v>103</v>
       </c>
-      <c r="B78" s="55"/>
-      <c r="C78" s="55"/>
-      <c r="D78" s="56"/>
-      <c r="E78" s="56"/>
-      <c r="F78" s="57"/>
-      <c r="G78" s="58"/>
-      <c r="H78" s="55"/>
-      <c r="I78" s="6"/>
-      <c r="J78" s="6"/>
-      <c r="K78" s="6"/>
-      <c r="L78" s="6"/>
-      <c r="M78" s="6"/>
-      <c r="N78" s="6"/>
-      <c r="O78" s="6"/>
-      <c r="P78" s="6"/>
-      <c r="Q78" s="6"/>
-      <c r="R78" s="6"/>
-      <c r="S78" s="6"/>
-      <c r="T78" s="6"/>
-      <c r="U78" s="6"/>
-      <c r="V78" s="6"/>
-      <c r="W78" s="6"/>
-      <c r="X78" s="6"/>
-      <c r="Y78" s="6"/>
-    </row>
-    <row r="79" spans="1:25" ht="15" customHeight="1">
-      <c r="A79" s="51" t="s">
-        <v>118</v>
-      </c>
-      <c r="B79" s="31" t="s">
-        <v>104</v>
-      </c>
-      <c r="C79" s="40" t="s">
-        <v>77</v>
-      </c>
-      <c r="D79" s="44">
-        <v>45315</v>
-      </c>
-      <c r="E79" s="44">
-        <v>45320</v>
-      </c>
-      <c r="F79" s="45">
-        <v>0</v>
-      </c>
-      <c r="G79" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="H79" s="40"/>
+      <c r="B79" s="55"/>
+      <c r="C79" s="55"/>
+      <c r="D79" s="56"/>
+      <c r="E79" s="56"/>
+      <c r="F79" s="57"/>
+      <c r="G79" s="58"/>
+      <c r="H79" s="55"/>
       <c r="I79" s="6"/>
-      <c r="J79" s="7"/>
-      <c r="K79" s="7"/>
-      <c r="L79" s="7"/>
-      <c r="M79" s="7"/>
-      <c r="N79" s="7"/>
-      <c r="O79" s="7"/>
-      <c r="P79" s="7"/>
-      <c r="Q79" s="7"/>
-      <c r="R79" s="7"/>
-      <c r="S79" s="7"/>
-      <c r="T79" s="7"/>
-      <c r="U79" s="7"/>
-      <c r="V79" s="7"/>
-      <c r="W79" s="7"/>
-      <c r="X79" s="7"/>
-      <c r="Y79" s="7"/>
+      <c r="J79" s="6"/>
+      <c r="K79" s="6"/>
+      <c r="L79" s="6"/>
+      <c r="M79" s="6"/>
+      <c r="N79" s="6"/>
+      <c r="O79" s="6"/>
+      <c r="P79" s="6"/>
+      <c r="Q79" s="6"/>
+      <c r="R79" s="6"/>
+      <c r="S79" s="6"/>
+      <c r="T79" s="6"/>
+      <c r="U79" s="6"/>
+      <c r="V79" s="6"/>
+      <c r="W79" s="6"/>
+      <c r="X79" s="6"/>
+      <c r="Y79" s="6"/>
     </row>
     <row r="80" spans="1:25" ht="15" customHeight="1">
       <c r="A80" s="51" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="B80" s="31" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C80" s="40" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="D80" s="44">
-        <v>45321</v>
+        <v>45315</v>
       </c>
       <c r="E80" s="44">
-        <v>45321</v>
+        <v>45320</v>
       </c>
       <c r="F80" s="45">
         <v>0</v>
@@ -2707,101 +2697,101 @@
       <c r="Y80" s="7"/>
     </row>
     <row r="81" spans="1:25" ht="15" customHeight="1">
-      <c r="A81" s="31"/>
-      <c r="B81" s="31"/>
-      <c r="C81" s="31"/>
-      <c r="D81" s="44"/>
-      <c r="E81" s="44"/>
-      <c r="F81" s="45"/>
-      <c r="G81" s="47"/>
-      <c r="H81" s="31"/>
-      <c r="I81" s="1"/>
+      <c r="A81" s="51" t="s">
+        <v>102</v>
+      </c>
+      <c r="B81" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="C81" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="D81" s="44">
+        <v>45321</v>
+      </c>
+      <c r="E81" s="44">
+        <v>45321</v>
+      </c>
+      <c r="F81" s="45">
+        <v>0</v>
+      </c>
+      <c r="G81" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="H81" s="40"/>
+      <c r="I81" s="6"/>
+      <c r="J81" s="7"/>
+      <c r="K81" s="7"/>
+      <c r="L81" s="7"/>
+      <c r="M81" s="7"/>
+      <c r="N81" s="7"/>
+      <c r="O81" s="7"/>
+      <c r="P81" s="7"/>
+      <c r="Q81" s="7"/>
+      <c r="R81" s="7"/>
+      <c r="S81" s="7"/>
+      <c r="T81" s="7"/>
+      <c r="U81" s="7"/>
+      <c r="V81" s="7"/>
+      <c r="W81" s="7"/>
+      <c r="X81" s="7"/>
+      <c r="Y81" s="7"/>
     </row>
     <row r="82" spans="1:25" ht="15" customHeight="1">
-      <c r="A82" s="54" t="s">
+      <c r="A82" s="31"/>
+      <c r="B82" s="31"/>
+      <c r="C82" s="31"/>
+      <c r="D82" s="44"/>
+      <c r="E82" s="44"/>
+      <c r="F82" s="45"/>
+      <c r="G82" s="47"/>
+      <c r="H82" s="31"/>
+      <c r="I82" s="1"/>
+    </row>
+    <row r="83" spans="1:25" ht="15" customHeight="1">
+      <c r="A83" s="54" t="s">
         <v>105</v>
       </c>
-      <c r="B82" s="55"/>
-      <c r="C82" s="55"/>
-      <c r="D82" s="56"/>
-      <c r="E82" s="56"/>
-      <c r="F82" s="57"/>
-      <c r="G82" s="58"/>
-      <c r="H82" s="55"/>
-      <c r="I82" s="6"/>
-      <c r="J82" s="6"/>
-      <c r="K82" s="6"/>
-      <c r="L82" s="6"/>
-      <c r="M82" s="6"/>
-      <c r="N82" s="6"/>
-      <c r="O82" s="6"/>
-      <c r="P82" s="6"/>
-      <c r="Q82" s="6"/>
-      <c r="R82" s="6"/>
-      <c r="S82" s="6"/>
-      <c r="T82" s="6"/>
-      <c r="U82" s="6"/>
-      <c r="V82" s="6"/>
-      <c r="W82" s="6"/>
-      <c r="X82" s="6"/>
-      <c r="Y82" s="6"/>
-    </row>
-    <row r="83" spans="1:25" ht="15" customHeight="1">
-      <c r="A83" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="B83" s="28" t="s">
+      <c r="B83" s="55"/>
+      <c r="C83" s="55"/>
+      <c r="D83" s="56"/>
+      <c r="E83" s="56"/>
+      <c r="F83" s="57"/>
+      <c r="G83" s="58"/>
+      <c r="H83" s="55"/>
+      <c r="I83" s="6"/>
+      <c r="J83" s="6"/>
+      <c r="K83" s="6"/>
+      <c r="L83" s="6"/>
+      <c r="M83" s="6"/>
+      <c r="N83" s="6"/>
+      <c r="O83" s="6"/>
+      <c r="P83" s="6"/>
+      <c r="Q83" s="6"/>
+      <c r="R83" s="6"/>
+      <c r="S83" s="6"/>
+      <c r="T83" s="6"/>
+      <c r="U83" s="6"/>
+      <c r="V83" s="6"/>
+      <c r="W83" s="6"/>
+      <c r="X83" s="6"/>
+      <c r="Y83" s="6"/>
+    </row>
+    <row r="84" spans="1:25" ht="15" customHeight="1">
+      <c r="A84" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="B84" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="C83" s="40" t="s">
+      <c r="C84" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="D83" s="59">
+      <c r="D84" s="59">
         <v>45323</v>
       </c>
-      <c r="E83" s="59">
+      <c r="E84" s="59">
         <v>45328</v>
-      </c>
-      <c r="F83" s="45">
-        <v>0</v>
-      </c>
-      <c r="G83" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="H83" s="40"/>
-      <c r="I83" s="6"/>
-      <c r="J83" s="7"/>
-      <c r="K83" s="7"/>
-      <c r="L83" s="7"/>
-      <c r="M83" s="7"/>
-      <c r="N83" s="7"/>
-      <c r="O83" s="7"/>
-      <c r="P83" s="7"/>
-      <c r="Q83" s="7"/>
-      <c r="R83" s="7"/>
-      <c r="S83" s="7"/>
-      <c r="T83" s="7"/>
-      <c r="U83" s="7"/>
-      <c r="V83" s="7"/>
-      <c r="W83" s="7"/>
-      <c r="X83" s="7"/>
-      <c r="Y83" s="7"/>
-    </row>
-    <row r="84" spans="1:25" ht="15" customHeight="1">
-      <c r="A84" s="40" t="s">
-        <v>106</v>
-      </c>
-      <c r="B84" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="C84" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="D84" s="59">
-        <v>45329</v>
-      </c>
-      <c r="E84" s="59">
-        <v>45329</v>
       </c>
       <c r="F84" s="45">
         <v>0</v>
@@ -2828,86 +2818,102 @@
       <c r="X84" s="7"/>
       <c r="Y84" s="7"/>
     </row>
-    <row r="85" spans="1:25">
-      <c r="A85" s="31"/>
-      <c r="B85" s="51"/>
-      <c r="C85" s="51"/>
-      <c r="D85" s="60"/>
-      <c r="E85" s="60"/>
-      <c r="F85" s="45"/>
-      <c r="G85" s="61"/>
-      <c r="H85" s="31"/>
-      <c r="I85" s="1"/>
+    <row r="85" spans="1:25" ht="15" customHeight="1">
+      <c r="A85" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="B85" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="C85" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="D85" s="59">
+        <v>45329</v>
+      </c>
+      <c r="E85" s="59">
+        <v>45329</v>
+      </c>
+      <c r="F85" s="45">
+        <v>0</v>
+      </c>
+      <c r="G85" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="H85" s="40"/>
+      <c r="I85" s="6"/>
+      <c r="J85" s="7"/>
+      <c r="K85" s="7"/>
+      <c r="L85" s="7"/>
+      <c r="M85" s="7"/>
+      <c r="N85" s="7"/>
+      <c r="O85" s="7"/>
+      <c r="P85" s="7"/>
+      <c r="Q85" s="7"/>
+      <c r="R85" s="7"/>
+      <c r="S85" s="7"/>
+      <c r="T85" s="7"/>
+      <c r="U85" s="7"/>
+      <c r="V85" s="7"/>
+      <c r="W85" s="7"/>
+      <c r="X85" s="7"/>
+      <c r="Y85" s="7"/>
     </row>
     <row r="86" spans="1:25">
-      <c r="A86" s="62" t="s">
+      <c r="A86" s="31"/>
+      <c r="B86" s="51"/>
+      <c r="C86" s="51"/>
+      <c r="D86" s="60"/>
+      <c r="E86" s="60"/>
+      <c r="F86" s="45"/>
+      <c r="G86" s="61"/>
+      <c r="H86" s="31"/>
+      <c r="I86" s="1"/>
+    </row>
+    <row r="87" spans="1:25">
+      <c r="A87" s="62" t="s">
         <v>107</v>
       </c>
-      <c r="B86" s="62"/>
-      <c r="C86" s="63"/>
-      <c r="D86" s="62"/>
-      <c r="E86" s="62"/>
-      <c r="F86" s="62"/>
-      <c r="G86" s="64"/>
-      <c r="H86" s="62"/>
-      <c r="I86" s="1"/>
-      <c r="J86" s="1"/>
-      <c r="K86" s="1"/>
-      <c r="L86" s="1"/>
-      <c r="M86" s="1"/>
-      <c r="N86" s="1"/>
-      <c r="O86" s="1"/>
-      <c r="P86" s="1"/>
-      <c r="Q86" s="1"/>
-      <c r="R86" s="1"/>
-      <c r="S86" s="1"/>
-      <c r="T86" s="1"/>
-      <c r="U86" s="1"/>
-      <c r="V86" s="1"/>
-      <c r="W86" s="1"/>
-      <c r="X86" s="1"/>
-      <c r="Y86" s="1"/>
-    </row>
-    <row r="87" spans="1:25" ht="15" customHeight="1">
-      <c r="A87" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="B87" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="C87" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="D87" s="59">
-        <v>45330</v>
-      </c>
-      <c r="E87" s="59">
-        <v>45332</v>
-      </c>
-      <c r="F87" s="45">
-        <v>0</v>
-      </c>
-      <c r="G87" s="47" t="s">
-        <v>85</v>
-      </c>
-      <c r="H87" s="31"/>
+      <c r="B87" s="62"/>
+      <c r="C87" s="63"/>
+      <c r="D87" s="62"/>
+      <c r="E87" s="62"/>
+      <c r="F87" s="62"/>
+      <c r="G87" s="64"/>
+      <c r="H87" s="62"/>
       <c r="I87" s="1"/>
+      <c r="J87" s="1"/>
+      <c r="K87" s="1"/>
+      <c r="L87" s="1"/>
+      <c r="M87" s="1"/>
+      <c r="N87" s="1"/>
+      <c r="O87" s="1"/>
+      <c r="P87" s="1"/>
+      <c r="Q87" s="1"/>
+      <c r="R87" s="1"/>
+      <c r="S87" s="1"/>
+      <c r="T87" s="1"/>
+      <c r="U87" s="1"/>
+      <c r="V87" s="1"/>
+      <c r="W87" s="1"/>
+      <c r="X87" s="1"/>
+      <c r="Y87" s="1"/>
     </row>
     <row r="88" spans="1:25" ht="15" customHeight="1">
       <c r="A88" s="31" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B88" s="31" t="s">
         <v>70</v>
       </c>
       <c r="C88" s="31" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
       <c r="D88" s="59">
-        <v>45333</v>
+        <v>45330</v>
       </c>
       <c r="E88" s="59">
-        <v>45336</v>
+        <v>45332</v>
       </c>
       <c r="F88" s="45">
         <v>0</v>
@@ -2920,19 +2926,19 @@
     </row>
     <row r="89" spans="1:25" ht="15" customHeight="1">
       <c r="A89" s="31" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B89" s="31" t="s">
         <v>70</v>
       </c>
       <c r="C89" s="31" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="D89" s="59">
-        <v>45337</v>
+        <v>45333</v>
       </c>
       <c r="E89" s="59">
-        <v>45341</v>
+        <v>45336</v>
       </c>
       <c r="F89" s="45">
         <v>0</v>
@@ -2945,19 +2951,19 @@
     </row>
     <row r="90" spans="1:25" ht="15" customHeight="1">
       <c r="A90" s="31" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B90" s="31" t="s">
         <v>70</v>
       </c>
       <c r="C90" s="31" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D90" s="59">
-        <v>45342</v>
+        <v>45337</v>
       </c>
       <c r="E90" s="59">
-        <v>45344</v>
+        <v>45341</v>
       </c>
       <c r="F90" s="45">
         <v>0</v>
@@ -2970,19 +2976,19 @@
     </row>
     <row r="91" spans="1:25" ht="15" customHeight="1">
       <c r="A91" s="31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B91" s="31" t="s">
         <v>70</v>
       </c>
       <c r="C91" s="31" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D91" s="59">
-        <v>45345</v>
+        <v>45342</v>
       </c>
       <c r="E91" s="59">
-        <v>45345</v>
+        <v>45344</v>
       </c>
       <c r="F91" s="45">
         <v>0</v>
@@ -2995,16 +3001,20 @@
     </row>
     <row r="92" spans="1:25" ht="15" customHeight="1">
       <c r="A92" s="31" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B92" s="31" t="s">
         <v>70</v>
       </c>
       <c r="C92" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="D92" s="44"/>
-      <c r="E92" s="44"/>
+        <v>115</v>
+      </c>
+      <c r="D92" s="59">
+        <v>45345</v>
+      </c>
+      <c r="E92" s="59">
+        <v>45345</v>
+      </c>
       <c r="F92" s="45">
         <v>0</v>
       </c>
@@ -3015,25 +3025,46 @@
       <c r="I92" s="1"/>
     </row>
     <row r="93" spans="1:25" ht="15" customHeight="1">
-      <c r="A93" s="65"/>
-      <c r="B93" s="65"/>
-      <c r="C93" s="65"/>
-      <c r="D93" s="65"/>
-      <c r="E93" s="65"/>
-      <c r="F93" s="65"/>
-      <c r="G93" s="65"/>
-      <c r="H93" s="65"/>
+      <c r="A93" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="B93" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="C93" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="D93" s="44"/>
+      <c r="E93" s="44"/>
+      <c r="F93" s="45">
+        <v>0</v>
+      </c>
+      <c r="G93" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="H93" s="31"/>
       <c r="I93" s="1"/>
     </row>
     <row r="94" spans="1:25" ht="15" customHeight="1">
-      <c r="A94" s="1"/>
-      <c r="B94" s="1"/>
-      <c r="C94" s="1"/>
-      <c r="D94" s="1"/>
-      <c r="E94" s="1"/>
-      <c r="F94" s="1"/>
-      <c r="G94" s="1"/>
-      <c r="H94" s="1"/>
+      <c r="A94" s="65"/>
+      <c r="B94" s="65"/>
+      <c r="C94" s="65"/>
+      <c r="D94" s="65"/>
+      <c r="E94" s="65"/>
+      <c r="F94" s="65"/>
+      <c r="G94" s="65"/>
+      <c r="H94" s="65"/>
+      <c r="I94" s="1"/>
+    </row>
+    <row r="95" spans="1:25" ht="15" customHeight="1">
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
+      <c r="C95" s="1"/>
+      <c r="D95" s="1"/>
+      <c r="E95" s="1"/>
+      <c r="F95" s="1"/>
+      <c r="G95" s="1"/>
+      <c r="H95" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>